<commit_message>
Add SIRT1 modeling project (iSIRT1_regulatoryModeling)
</commit_message>
<xml_diff>
--- a/retinopathyMouseModeling/Data/Retina_mets.xlsx
+++ b/retinopathyMouseModeling/Data/Retina_mets.xlsx
@@ -23914,8 +23914,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000914F637700DE8469E60BD164038A335" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95a6e8769c437caeaa6b68c3874ffbfe">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="53de05c8-a8b0-4009-b9d3-18284b78ab9e" xmlns:ns3="b5437027-0024-4447-881e-b1af9f72c9dc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff04aabef00aaebe0dbe838155a24aa9" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000914F637700DE8469E60BD164038A335" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5d7e79cc08e50437b6860aef4e08d083">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="53de05c8-a8b0-4009-b9d3-18284b78ab9e" xmlns:ns3="b5437027-0024-4447-881e-b1af9f72c9dc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="097adb27deb1439976489058284dc125" ns2:_="" ns3:_="">
     <xsd:import namespace="53de05c8-a8b0-4009-b9d3-18284b78ab9e"/>
     <xsd:import namespace="b5437027-0024-4447-881e-b1af9f72c9dc"/>
     <xsd:element name="properties">
@@ -23937,6 +23937,7 @@
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -23957,7 +23958,7 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="11" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="1d417cb3-2750-492f-8db0-46aaf8d22b50" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="11" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="1d417cb3-2750-492f-8db0-46aaf8d22b50" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -24001,6 +24002,11 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="22" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b5437027-0024-4447-881e-b1af9f72c9dc" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -24016,7 +24022,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -24035,7 +24041,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -24052,8 +24058,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -24163,7 +24169,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91C80FA3-D70D-4325-9945-DCEDEC0BD441}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87BB4AF5-7437-4FB6-87F7-4E3BAFD25384}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>